<commit_message>
CV Pantallde retención, reportes
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-Retenciones.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-Retenciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B206E48-34D9-EE4A-9E18-EE987BD4AB90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5258E8C5-5717-EA43-ACA4-364094CCE01E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="3460" windowWidth="38540" windowHeight="22340" xr2:uid="{306FDEFB-6B54-2B40-874B-FA2C57B165FD}"/>
+    <workbookView xWindow="20280" yWindow="13900" windowWidth="38540" windowHeight="22340" xr2:uid="{306FDEFB-6B54-2B40-874B-FA2C57B165FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>ESTABLECIMIENTO :</t>
   </si>
@@ -42,12 +42,6 @@
     <t>FECHA</t>
   </si>
   <si>
-    <t># FACT</t>
-  </si>
-  <si>
-    <t>RUC / CI</t>
-  </si>
-  <si>
     <t>PROVEEDOR</t>
   </si>
   <si>
@@ -57,40 +51,22 @@
     <t>ESTADO</t>
   </si>
   <si>
-    <t>COD</t>
-  </si>
-  <si>
-    <t>DETALLE</t>
-  </si>
-  <si>
-    <t># COMPROBANTE</t>
-  </si>
-  <si>
-    <t>AUTORIZACIÓN</t>
-  </si>
-  <si>
-    <t>AÑO</t>
-  </si>
-  <si>
-    <t>MES</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
-    <t>IMPUESTO</t>
-  </si>
-  <si>
-    <t>BASE IMPONIBLE</t>
-  </si>
-  <si>
-    <t>% RETENCIÓN</t>
-  </si>
-  <si>
     <t>LISTA RETENCIONES</t>
   </si>
   <si>
-    <t>RETENCIÓN</t>
+    <t>#COMPROBANTE</t>
+  </si>
+  <si>
+    <t>RUC</t>
+  </si>
+  <si>
+    <t>DOC ASOCIADO</t>
+  </si>
+  <si>
+    <t>PERIODO</t>
   </si>
 </sst>
 </file>
@@ -179,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -192,9 +168,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -204,8 +179,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,102 +493,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A527F97D-E6F1-DE46-8C92-B6BC6FE0A79B}">
-  <dimension ref="A2:P11"/>
+  <dimension ref="A2:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G4"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="6" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="33.33203125" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -625,88 +587,45 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="E9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="E11" s="11"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E10" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="L9:P9"/>
+  <mergeCells count="5">
+    <mergeCell ref="A2:J2"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B6:G6"/>

</xml_diff>